<commit_message>
New protocol added for distributing stock solutions to two destination plates. Needs to be modified so that the information is not hard-coded. Consider updating the protocol to distribute a single stock solution across two or more destination plates.
</commit_message>
<xml_diff>
--- a/data/1-SAMPLE_DATA-ER.xlsx
+++ b/data/1-SAMPLE_DATA-ER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pinkp\GitHub\opentrons\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2D7569-776D-4284-A09F-B9E72E342571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6EA7B8-37AC-469B-9939-438800D44FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{319A77C1-AB08-46A6-8832-F6BE764A2789}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{319A77C1-AB08-46A6-8832-F6BE764A2789}"/>
   </bookViews>
   <sheets>
     <sheet name="Dispense_Volumes" sheetId="1" r:id="rId1"/>
@@ -101,21 +101,9 @@
     <t>A5</t>
   </si>
   <si>
-    <t xml:space="preserve">Labware  </t>
-  </si>
-  <si>
     <t>Labware_API_name</t>
   </si>
   <si>
-    <t>Labware_Role</t>
-  </si>
-  <si>
-    <t>Tips used</t>
-  </si>
-  <si>
-    <t>Destination wells</t>
-  </si>
-  <si>
     <t>Labware_Deck_Slot</t>
   </si>
   <si>
@@ -125,9 +113,6 @@
     <t>p300_single_gen2</t>
   </si>
   <si>
-    <t>Stock Solutions</t>
-  </si>
-  <si>
     <t>NEST 96 Well Plate 100 µL PCR Full Skirt</t>
   </si>
   <si>
@@ -162,6 +147,21 @@
   </si>
   <si>
     <t>B2</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Destination_Wells</t>
+  </si>
+  <si>
+    <t>Stock_Solutions</t>
+  </si>
+  <si>
+    <t>Tips_Rack</t>
   </si>
 </sst>
 </file>
@@ -205,26 +205,28 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -247,24 +249,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,7 +582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A62E9950-ECF7-43D6-9953-F32FAF587F46}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -590,7 +593,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>7</v>
@@ -802,7 +805,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -886,7 +889,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -897,7 +900,7 @@
         <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -909,7 +912,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F235A423-AD2F-4355-A262-4EEC2C9169F5}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -919,74 +924,74 @@
     <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>25</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="C1" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="D1" s="7" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>24</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>24</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
+      <c r="B4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
+      <c r="B5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1009,24 +1014,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>